<commit_message>
create new and correct add_to functions
</commit_message>
<xml_diff>
--- a/notebooks/stations_name_ref.xlsx
+++ b/notebooks/stations_name_ref.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B152"/>
+  <dimension ref="A1:C153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,1816 +444,2593 @@
           <t>ref</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>route_name_list</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Vlaardingen West</t>
+          <t>Isolatorweg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Vlaardingen Centrum</t>
+          <t>Station Sloterdijk</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Vlaardingen Oost</t>
+          <t>De Vlugtlaan</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Schiedam Nieuwland</t>
+          <t>Jan van Galenstraat</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Schiedam Centrum</t>
+          <t>Postjesweg</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Marconiplein</t>
+          <t>Lelylaan</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Delfshaven</t>
+          <t>Heemstedestraat</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Coolhaven</t>
+          <t>Henk Sneevlietweg</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dijkzigt</t>
+          <t>Amstelveenseweg</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Eendrachtsplein</t>
+          <t>Zuid</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Beurs</t>
+          <t>Station RAI</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A, B, C, D, E</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Blaak</t>
+          <t>Overamstel</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Oostplein</t>
+          <t>Van der Madeweg</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Gerdesiaweg</t>
+          <t>Duivendrecht</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Voorschoterlaan</t>
+          <t>Strandvliet</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kralingse Zoom</t>
+          <t>Bijlmer ArenA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Capelsebrug</t>
+          <t>Bullewijk</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Schenkel</t>
+          <t>Holendrecht</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Prinsenlaan</t>
+          <t>Reigersbos</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Oosterflank</t>
+          <t>Gein</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Metro 50: Gein =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Gein</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Graskruid</t>
+          <t>Reigersbos</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Romeynshof</t>
+          <t>Holendrecht</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Binnenhof</t>
+          <t>Bullewijk</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Binnenhof</t>
+          <t>Bijlmer ArenA</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Romeynshof</t>
+          <t>Strandvliet</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Graskruid</t>
+          <t>Duivendrecht</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Van der Madeweg</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Oosterflank</t>
+          <t>Overamstel</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Prinsenlaan</t>
+          <t>Station RAI</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Schenkel</t>
+          <t>Zuid</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Capelsebrug</t>
+          <t>Amstelveenseweg</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Kralingse Zoom</t>
+          <t>Henk Sneevlietweg</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Voorschoterlaan</t>
+          <t>Heemstedestraat</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Gerdesiaweg</t>
+          <t>Lelylaan</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Oostplein</t>
+          <t>Postjesweg</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Blaak</t>
+          <t>Jan van Galenstraat</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Beurs</t>
+          <t>De Vlugtlaan</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>A, B, C, D, E</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Eendrachtsplein</t>
+          <t>Station Sloterdijk</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Dijkzigt</t>
+          <t>Isolatorweg</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Metro 50: Isolatorweg =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Coolhaven</t>
+          <t>Isolatorweg</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Delfshaven</t>
+          <t>Station Sloterdijk</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Marconiplein</t>
+          <t>De Vlugtlaan</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Schiedam Centrum</t>
+          <t>Jan van Galenstraat</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Schiedam Nieuwland</t>
+          <t>Postjesweg</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Vlaardingen Oost</t>
+          <t>Lelylaan</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Vlaardingen Centrum</t>
+          <t>Heemstedestraat</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Hoek van Holland Strand</t>
+          <t>Henk Sneevlietweg</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Hoek van Holland Haven</t>
+          <t>Amstelveenseweg</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Steendijkpolder</t>
+          <t>Zuid</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Maassluis West</t>
+          <t>Station RAI</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Maassluis Centrum</t>
+          <t>Wibautstraat</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Vlaardingen West</t>
+          <t>Weesperplein</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Hesseplaats</t>
+          <t>Waterlooplein</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Nieuw Verlaat</t>
+          <t>Nieuwmarkt</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Ambachtsland</t>
+          <t>Centraal Station</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>De Tochten</t>
+          <t>Amstelstation</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Nesselande</t>
+          <t>Spaklerweg</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Nesselande</t>
+          <t>Overamstel</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>De Tochten</t>
+          <t>Centraal Station</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Ambachtsland</t>
+          <t>Nieuwmarkt</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Nieuw Verlaat</t>
+          <t>Waterlooplein</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Hesseplaats</t>
+          <t>Weesperplein</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Vlaardingen West</t>
+          <t>Wibautstraat</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Maassluis Centrum</t>
+          <t>Amstelstation</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Maassluis West</t>
+          <t>Spaklerweg</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Steendijkpolder</t>
+          <t>Overamstel</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Hoek van Holland Haven</t>
+          <t>Station RAI</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Hoek van Holland Strand</t>
+          <t>Zuid</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>De Terp</t>
+          <t>Amstelveenseweg</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Capelle Centrum</t>
+          <t>Henk Sneevlietweg</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Slotlaan</t>
+          <t>Heemstedestraat</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Schiedam Centrum</t>
+          <t>Lelylaan</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Parkweg</t>
+          <t>Postjesweg</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Troelstralaan</t>
+          <t>Jan van Galenstraat</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Vijfsluizen</t>
+          <t>De Vlugtlaan</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Pernis</t>
+          <t>Station Sloterdijk</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Tussenwater</t>
+          <t>Isolatorweg</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Hoogvliet</t>
+          <t>Zuid</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Metro 52: Noord =&gt; Zuid</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Zalmplaat</t>
+          <t>Europaplein</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Metro 52: Noord =&gt; Zuid</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Spijkenisse Centrum</t>
+          <t>De Pijp</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Metro 52: Noord =&gt; Zuid</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Heemraadlaan</t>
+          <t>Vijzelgracht</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Metro 52: Noord =&gt; Zuid</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>De Akkers</t>
+          <t>Rokin</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Metro 52: Noord =&gt; Zuid</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>De Akkers</t>
+          <t>Centraal Station</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Metro 52: Noord =&gt; Zuid</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Heemraadlaan</t>
+          <t>Noorderpark</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Metro 52: Noord =&gt; Zuid</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Spijkenisse Centrum</t>
+          <t>Noord</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Metro 52: Noord =&gt; Zuid</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Zalmplaat</t>
+          <t>Noord</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Metro 52: Zuid =&gt; Noord</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Hoogvliet</t>
+          <t>Noorderpark</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Metro 52: Zuid =&gt; Noord</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Tussenwater</t>
+          <t>Centraal Station</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Metro 52: Zuid =&gt; Noord</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Pernis</t>
+          <t>Rokin</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Metro 52: Zuid =&gt; Noord</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Vijfsluizen</t>
+          <t>Vijzelgracht</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Metro 52: Zuid =&gt; Noord</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Troelstralaan</t>
+          <t>De Pijp</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Metro 52: Zuid =&gt; Noord</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Parkweg</t>
+          <t>Europaplein</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Metro 52: Zuid =&gt; Noord</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Capelsebrug</t>
+          <t>Zuid</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>A, B, C</t>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Metro 52: Zuid =&gt; Noord</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Slotlaan</t>
+          <t>Gaasperplas</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Capelle Centrum</t>
+          <t>Kraaiennest</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>De Terp</t>
+          <t>Ganzenhoef</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Rotterdam Centraal</t>
+          <t>Verrijn Stuartweg</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Stadhuis</t>
+          <t>Station Diemen Zuid</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Beurs</t>
+          <t>Venserpolder</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>A, B, C, D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Leuvehaven</t>
+          <t>Van der Madeweg</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Wilhelminaplein</t>
+          <t>Spaklerweg</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Rijnhaven</t>
+          <t>Amstelstation</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Maashaven</t>
+          <t>Wibautstraat</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Zuidplein</t>
+          <t>Weesperplein</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Slinge</t>
+          <t>Waterlooplein</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Rhoon</t>
+          <t>Nieuwmarkt</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Poortugaal</t>
+          <t>Centraal Station</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Tussenwater</t>
+          <t>Centraal Station</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Tussenwater</t>
+          <t>Nieuwmarkt</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>C, D</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Poortugaal</t>
+          <t>Waterlooplein</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Rhoon</t>
+          <t>Weesperplein</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Slinge</t>
+          <t>Wibautstraat</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Zuidplein</t>
+          <t>Amstelstation</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Maashaven</t>
+          <t>Spaklerweg</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Rijnhaven</t>
+          <t>Van der Madeweg</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Wilhelminaplein</t>
+          <t>Venserpolder</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Leuvehaven</t>
+          <t>Station Diemen Zuid</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Beurs</t>
+          <t>Verrijn Stuartweg</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>A, B, C, D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Stadhuis</t>
+          <t>Ganzenhoef</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Slinge</t>
+          <t>Kraaiennest</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Rotterdam Centraal</t>
+          <t>Gaasperplas</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Blijdorp</t>
+          <t>Gein</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Melanchthonweg</t>
+          <t>Reigersbos</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Meijersplein / Airport</t>
+          <t>Holendrecht</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Rodenrijs</t>
+          <t>Bullewijk</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Berkel Westpolder</t>
+          <t>Bijlmer ArenA</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Pijnacker Zuid</t>
+          <t>Strandvliet</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Pijnacker Centrum</t>
+          <t>Duivendrecht</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Nootdorp</t>
+          <t>Van der Madeweg</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Leidschenveen</t>
+          <t>Spaklerweg</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Forepark</t>
+          <t>Amstelstation</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Leidschendam-Voorburg</t>
+          <t>Wibautstraat</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Voorburg 't Loo</t>
+          <t>Weesperplein</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Den Haag Laan van NOI</t>
+          <t>Waterlooplein</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Den Haag Centraal</t>
+          <t>Nieuwmarkt</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Den Haag Centraal</t>
+          <t>Centraal Station</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Metro 54: Centraal Station =&gt; Gein</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Den Haag Laan van NOI</t>
+          <t>Centraal Station</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Voorburg 't Loo</t>
+          <t>Nieuwmarkt</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Leidschendam-Voorburg</t>
+          <t>Waterlooplein</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Forepark</t>
+          <t>Weesperplein</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Leidschenveen</t>
+          <t>Wibautstraat</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Nootdorp</t>
+          <t>Amstelstation</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Pijnacker Centrum</t>
+          <t>Spaklerweg</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Pijnacker Zuid</t>
+          <t>Van der Madeweg</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Berkel Westpolder</t>
+          <t>Duivendrecht</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Rodenrijs</t>
+          <t>Strandvliet</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Meijersplein / Airport</t>
+          <t>Bijlmer ArenA</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Melanchthonweg</t>
+          <t>Bullewijk</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Blijdorp</t>
+          <t>Holendrecht</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Rotterdam Centraal</t>
+          <t>Reigersbos</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>D, E</t>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Gein</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Metro 54: Gein =&gt; Centraal Station</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
clear transfer1_ & transfer.py
</commit_message>
<xml_diff>
--- a/notebooks/stations_name_ref.xlsx
+++ b/notebooks/stations_name_ref.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C153"/>
+  <dimension ref="A1:B245"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,2593 +444,2932 @@
           <t>ref</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>route_name_list</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Isolatorweg</t>
+          <t>Vlaardingen West</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Station Sloterdijk</t>
+          <t>Vlaardingen Centrum</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>De Vlugtlaan</t>
+          <t>Vlaardingen Oost</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jan van Galenstraat</t>
+          <t>Schiedam Nieuwland</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Postjesweg</t>
+          <t>Schiedam Centrum</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Lelylaan</t>
+          <t>Marconiplein</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Heemstedestraat</t>
+          <t>Delfshaven</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Henk Sneevlietweg</t>
+          <t>Coolhaven</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Amstelveenseweg</t>
+          <t>Dijkzigt</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Zuid</t>
+          <t>Eendrachtsplein</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Station RAI</t>
+          <t>Beurs</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Overamstel</t>
+          <t>Blaak</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Van der Madeweg</t>
+          <t>Oostplein</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Duivendrecht</t>
+          <t>Gerdesiaweg</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Strandvliet</t>
+          <t>Voorschoterlaan</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bijlmer ArenA</t>
+          <t>Kralingse Zoom</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bullewijk</t>
+          <t>Capelsebrug</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Holendrecht</t>
+          <t>Schenkel</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Reigersbos</t>
+          <t>Prinsenlaan</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Gein</t>
+          <t>Oosterflank</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Metro 50: Gein =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Gein</t>
+          <t>Alexander</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Reigersbos</t>
+          <t>Graskruid</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Holendrecht</t>
+          <t>Romeynshof</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Bullewijk</t>
+          <t>Binnenhof</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Bijlmer ArenA</t>
+          <t>Binnenhof</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Strandvliet</t>
+          <t>Romeynshof</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Duivendrecht</t>
+          <t>Graskruid</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Van der Madeweg</t>
+          <t>Alexander</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Overamstel</t>
+          <t>Oosterflank</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Station RAI</t>
+          <t>Prinsenlaan</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Zuid</t>
+          <t>Schenkel</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Amstelveenseweg</t>
+          <t>Capelsebrug</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Henk Sneevlietweg</t>
+          <t>Kralingse Zoom</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Heemstedestraat</t>
+          <t>Voorschoterlaan</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Lelylaan</t>
+          <t>Gerdesiaweg</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Postjesweg</t>
+          <t>Oostplein</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Jan van Galenstraat</t>
+          <t>Blaak</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>De Vlugtlaan</t>
+          <t>Beurs</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Station Sloterdijk</t>
+          <t>Eendrachtsplein</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Isolatorweg</t>
+          <t>Dijkzigt</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Metro 50: Isolatorweg =&gt; Gein</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Isolatorweg</t>
+          <t>Coolhaven</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Station Sloterdijk</t>
+          <t>Delfshaven</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>De Vlugtlaan</t>
+          <t>Marconiplein</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Jan van Galenstraat</t>
+          <t>Schiedam Centrum</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Postjesweg</t>
+          <t>Schiedam Nieuwland</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Lelylaan</t>
+          <t>Vlaardingen Oost</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Heemstedestraat</t>
+          <t>Vlaardingen Centrum</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Henk Sneevlietweg</t>
+          <t>Vlaardingen West</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Amstelveenseweg</t>
+          <t>Hoek van Holland Strand</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Zuid</t>
+          <t>Hoek van Holland Haven</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Station RAI</t>
+          <t>Steendijkpolder</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Wibautstraat</t>
+          <t>Maassluis West</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Weesperplein</t>
+          <t>Maassluis Centrum</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Waterlooplein</t>
+          <t>Vlaardingen West</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Nieuwmarkt</t>
+          <t>Vlaardingen Centrum</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Centraal Station</t>
+          <t>Vlaardingen Oost</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Amstelstation</t>
+          <t>Schiedam Nieuwland</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Spaklerweg</t>
+          <t>Schiedam Centrum</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Overamstel</t>
+          <t>Marconiplein</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Metro 51: Centraal Station =&gt; Isolatorweg</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Centraal Station</t>
+          <t>Delfshaven</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Nieuwmarkt</t>
+          <t>Coolhaven</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Waterlooplein</t>
+          <t>Dijkzigt</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Weesperplein</t>
+          <t>Eendrachtsplein</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Wibautstraat</t>
+          <t>Beurs</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Amstelstation</t>
+          <t>Blaak</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Spaklerweg</t>
+          <t>Oostplein</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Overamstel</t>
+          <t>Gerdesiaweg</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Station RAI</t>
+          <t>Voorschoterlaan</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Zuid</t>
+          <t>Kralingse Zoom</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Amstelveenseweg</t>
+          <t>Capelsebrug</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Henk Sneevlietweg</t>
+          <t>Schenkel</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Heemstedestraat</t>
+          <t>Prinsenlaan</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Lelylaan</t>
+          <t>Oosterflank</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Postjesweg</t>
+          <t>Alexander</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Jan van Galenstraat</t>
+          <t>Graskruid</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>De Vlugtlaan</t>
+          <t>Hesseplaats</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Station Sloterdijk</t>
+          <t>Nieuw Verlaat</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Isolatorweg</t>
+          <t>Ambachtsland</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Metro 51: Isolatorweg =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Zuid</t>
+          <t>De Tochten</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Metro 52: Noord =&gt; Zuid</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Europaplein</t>
+          <t>Nesselande</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Metro 52: Noord =&gt; Zuid</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>De Pijp</t>
+          <t>Nesselande</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Metro 52: Noord =&gt; Zuid</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Vijzelgracht</t>
+          <t>De Tochten</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Metro 52: Noord =&gt; Zuid</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Rokin</t>
+          <t>Ambachtsland</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Metro 52: Noord =&gt; Zuid</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Centraal Station</t>
+          <t>Nieuw Verlaat</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Metro 52: Noord =&gt; Zuid</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Noorderpark</t>
+          <t>Hesseplaats</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Metro 52: Noord =&gt; Zuid</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Noord</t>
+          <t>Graskruid</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Metro 52: Noord =&gt; Zuid</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Noord</t>
+          <t>Alexander</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Metro 52: Zuid =&gt; Noord</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Noorderpark</t>
+          <t>Oosterflank</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Metro 52: Zuid =&gt; Noord</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Centraal Station</t>
+          <t>Prinsenlaan</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Metro 52: Zuid =&gt; Noord</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Rokin</t>
+          <t>Schenkel</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Metro 52: Zuid =&gt; Noord</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Vijzelgracht</t>
+          <t>Capelsebrug</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Metro 52: Zuid =&gt; Noord</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>De Pijp</t>
+          <t>Kralingse Zoom</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Metro 52: Zuid =&gt; Noord</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Europaplein</t>
+          <t>Voorschoterlaan</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Metro 52: Zuid =&gt; Noord</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Zuid</t>
+          <t>Gerdesiaweg</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Metro 52: Zuid =&gt; Noord</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Gaasperplas</t>
+          <t>Oostplein</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Kraaiennest</t>
+          <t>Blaak</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Ganzenhoef</t>
+          <t>Beurs</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Verrijn Stuartweg</t>
+          <t>Eendrachtsplein</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Station Diemen Zuid</t>
+          <t>Dijkzigt</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Venserpolder</t>
+          <t>Coolhaven</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Van der Madeweg</t>
+          <t>Delfshaven</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Spaklerweg</t>
+          <t>Marconiplein</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Amstelstation</t>
+          <t>Schiedam Centrum</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Wibautstraat</t>
+          <t>Schiedam Nieuwland</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Weesperplein</t>
+          <t>Vlaardingen Oost</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Waterlooplein</t>
+          <t>Vlaardingen Centrum</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Nieuwmarkt</t>
+          <t>Vlaardingen West</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Centraal Station</t>
+          <t>Maassluis Centrum</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Metro 53: Centraal Station =&gt; Gaasperplas</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Centraal Station</t>
+          <t>Maassluis West</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Nieuwmarkt</t>
+          <t>Steendijkpolder</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Waterlooplein</t>
+          <t>Hoek van Holland Haven</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Weesperplein</t>
+          <t>Hoek van Holland Strand</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Wibautstraat</t>
+          <t>De Terp</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Amstelstation</t>
+          <t>Capelle Centrum</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Spaklerweg</t>
+          <t>Slotlaan</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Van der Madeweg</t>
+          <t>Capelsebrug</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Venserpolder</t>
+          <t>Kralingse Zoom</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Station Diemen Zuid</t>
+          <t>Voorschoterlaan</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Verrijn Stuartweg</t>
+          <t>Gerdesiaweg</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Ganzenhoef</t>
+          <t>Oostplein</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Kraaiennest</t>
+          <t>Blaak</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Gaasperplas</t>
+          <t>Beurs</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Metro 53: Gaasperplas =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Gein</t>
+          <t>Eendrachtsplein</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Reigersbos</t>
+          <t>Dijkzigt</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Holendrecht</t>
+          <t>Coolhaven</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Bullewijk</t>
+          <t>Delfshaven</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Bijlmer ArenA</t>
+          <t>Marconiplein</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Strandvliet</t>
+          <t>Schiedam Centrum</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Duivendrecht</t>
+          <t>Parkweg</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Van der Madeweg</t>
+          <t>Troelstralaan</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Spaklerweg</t>
+          <t>Vijfsluizen</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Amstelstation</t>
+          <t>Pernis</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Wibautstraat</t>
+          <t>Tussenwater</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Weesperplein</t>
+          <t>Hoogvliet</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Waterlooplein</t>
+          <t>Zalmplaat</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Nieuwmarkt</t>
+          <t>Spijkenisse Centrum</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Centraal Station</t>
+          <t>Heemraadlaan</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>Metro 54: Centraal Station =&gt; Gein</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Centraal Station</t>
+          <t>De Akkers</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Nieuwmarkt</t>
+          <t>De Akkers</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Waterlooplein</t>
+          <t>Heemraadlaan</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Weesperplein</t>
+          <t>Spijkenisse Centrum</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Wibautstraat</t>
+          <t>Zalmplaat</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Amstelstation</t>
+          <t>Hoogvliet</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Spaklerweg</t>
+          <t>Tussenwater</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Van der Madeweg</t>
+          <t>Pernis</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Duivendrecht</t>
+          <t>Vijfsluizen</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Strandvliet</t>
+          <t>Troelstralaan</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Bijlmer ArenA</t>
+          <t>Parkweg</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Bullewijk</t>
+          <t>Schiedam Centrum</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Holendrecht</t>
+          <t>Marconiplein</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Reigersbos</t>
+          <t>Delfshaven</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Gein</t>
+          <t>Coolhaven</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>Metro 54: Gein =&gt; Centraal Station</t>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Dijkzigt</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Eendrachtsplein</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Beurs</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Blaak</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Oostplein</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Gerdesiaweg</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Voorschoterlaan</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Kralingse Zoom</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Capelsebrug</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Slotlaan</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Capelle Centrum</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>De Terp</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Rotterdam Centraal</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Stadhuis</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Beurs</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Leuvehaven</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Wilhelminaplein</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Rijnhaven</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Maashaven</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Zuidplein</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Slinge</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Rhoon</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Poortugaal</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Tussenwater</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Hoogvliet</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Zalmplaat</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Spijkenisse Centrum</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Heemraadlaan</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>De Akkers</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>De Akkers</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Heemraadlaan</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Spijkenisse Centrum</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Zalmplaat</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Hoogvliet</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Tussenwater</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Poortugaal</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Rhoon</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Slinge</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Zuidplein</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Maashaven</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Rijnhaven</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Wilhelminaplein</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Leuvehaven</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Beurs</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Stadhuis</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Rotterdam Centraal</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Slinge</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Zuidplein</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Maashaven</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Rijnhaven</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Wilhelminaplein</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Leuvehaven</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Beurs</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Stadhuis</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Rotterdam Centraal</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Blijdorp</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Melanchthonweg</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Meijersplein / Airport</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Rodenrijs</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Berkel Westpolder</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Pijnacker Zuid</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Pijnacker Centrum</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Nootdorp</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Leidschenveen</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Forepark</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Leidschendam-Voorburg</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Voorburg 't Loo</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Den Haag Laan van NOI</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Den Haag Centraal</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Den Haag Centraal</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Den Haag Laan van NOI</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Voorburg 't Loo</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Leidschendam-Voorburg</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Forepark</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Leidschenveen</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Nootdorp</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Pijnacker Centrum</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Pijnacker Zuid</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Berkel Westpolder</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Rodenrijs</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Meijersplein / Airport</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Melanchthonweg</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Blijdorp</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Rotterdam Centraal</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Stadhuis</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Beurs</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Leuvehaven</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Wilhelminaplein</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Rijnhaven</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Maashaven</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Zuidplein</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Slinge</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>E</t>
         </is>
       </c>
     </row>

</xml_diff>